<commit_message>
Agregar nuevas bases de datos
</commit_message>
<xml_diff>
--- a/DataBase/Iris/calculosIris.xlsx
+++ b/DataBase/Iris/calculosIris.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melencino\Documents\Universidad\semestre_22-1\RP\RP-22-1\DocumentosIris\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melencino\Documents\Universidad\semestre_22-1\RP\RP-22-1\DataBase\Iris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050F4275-08B3-49BE-B254-2DDA4ACA5041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E033F41-1B26-4FAF-806E-1060C8E8EE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="975" windowWidth="12675" windowHeight="6000" xr2:uid="{CCA8BA67-BBC2-479E-9B84-1D661240B96A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{CCA8BA67-BBC2-479E-9B84-1D661240B96A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="29">
   <si>
     <t>Iris-setosa</t>
   </si>
@@ -65,12 +65,60 @@
   <si>
     <t>Calcular Distancia:</t>
   </si>
+  <si>
+    <t>entrenamientos -&gt; minDistancia.entrenar();</t>
+  </si>
+  <si>
+    <t>150 -&gt; entrenamiento</t>
+  </si>
+  <si>
+    <t>Otro archivo -&gt; diferente</t>
+  </si>
+  <si>
+    <t>clasificar -&gt; minDistacia.clasificar();</t>
+  </si>
+  <si>
+    <t>Patron -&gt; vector, clase</t>
+  </si>
+  <si>
+    <t>Txt1 -&gt; Herramientas.instancias;</t>
+  </si>
+  <si>
+    <t>Txt2 -&gt; Herramientas.instancias;</t>
+  </si>
+  <si>
+    <t>5, 8, 9, 2, Versicolor, Virginica</t>
+  </si>
+  <si>
+    <t>Setosa</t>
+  </si>
+  <si>
+    <t>Versicolor</t>
+  </si>
+  <si>
+    <t>Virginica</t>
+  </si>
+  <si>
+    <t>Matriz</t>
+  </si>
+  <si>
+    <t>Originales</t>
+  </si>
+  <si>
+    <t>Resultantes</t>
+  </si>
+  <si>
+    <t>5, 8, 9, 2, Versicolor, setosa</t>
+  </si>
+  <si>
+    <t>5, 8, 9, 2, Versicolor, versicolor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,8 +126,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,6 +255,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -265,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -297,6 +376,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -312,10 +395,16 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -325,10 +414,10 @@
   <colors>
     <mruColors>
       <color rgb="FF5FDB5F"/>
+      <color rgb="FFD69298"/>
       <color rgb="FF67B9D3"/>
       <color rgb="FFC05862"/>
       <color rgb="FFE3B3B8"/>
-      <color rgb="FFD69298"/>
       <color rgb="FF96DBDE"/>
     </mruColors>
   </colors>
@@ -640,23 +729,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A2A42C-D3AD-4B48-866F-74A22BBAD4B6}">
-  <dimension ref="A1:M150"/>
+  <dimension ref="A1:P150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="42.42578125" customWidth="1"/>
     <col min="8" max="8" width="21.42578125" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="12" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
     <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -673,7 +766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>4.9000000000000004</v>
       </c>
@@ -689,8 +782,11 @@
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4.7</v>
       </c>
@@ -706,17 +802,17 @@
       <c r="E3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="L3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4.5999999999999996</v>
       </c>
@@ -732,27 +828,30 @@
       <c r="E4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="13">
+      <c r="G4" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="13">
         <f>SUM(A1:A50)</f>
         <v>250.29999999999998</v>
       </c>
-      <c r="J4" s="13">
+      <c r="M4" s="13">
         <f>SUM(B1:B50)</f>
         <v>170.90000000000003</v>
       </c>
-      <c r="K4" s="13">
+      <c r="N4" s="13">
         <f>SUM(C1:C50)</f>
         <v>73.2</v>
       </c>
-      <c r="L4" s="13">
+      <c r="O4" s="13">
         <f>SUM(D1:D50)</f>
         <v>12.199999999999996</v>
       </c>
-      <c r="M4" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P4" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -768,27 +867,30 @@
       <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="13">
+      <c r="G5" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="13">
         <f>SUM(A51:A100)</f>
         <v>296.8</v>
       </c>
-      <c r="J5" s="13">
+      <c r="M5" s="13">
         <f>SUM(B51:B100)</f>
         <v>138.50000000000003</v>
       </c>
-      <c r="K5" s="13">
+      <c r="N5" s="13">
         <f>SUM(C51:C100)</f>
         <v>212.99999999999997</v>
       </c>
-      <c r="L5" s="13">
+      <c r="O5" s="13">
         <f>SUM(D51:D100)</f>
         <v>66.3</v>
       </c>
-      <c r="M5" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P5" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5.4</v>
       </c>
@@ -804,27 +906,27 @@
       <c r="E6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="13">
+      <c r="L6" s="13">
         <f>SUM(A101:A150)</f>
         <v>329.39999999999992</v>
       </c>
-      <c r="J6" s="13">
+      <c r="M6" s="13">
         <f>SUM(B101:B150)</f>
         <v>148.69999999999999</v>
       </c>
-      <c r="K6" s="13">
+      <c r="N6" s="13">
         <f>SUM(C101:C150)</f>
         <v>277.59999999999997</v>
       </c>
-      <c r="L6" s="13">
+      <c r="O6" s="13">
         <f>SUM(D100:D150)</f>
         <v>102.59999999999998</v>
       </c>
-      <c r="M6" s="12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P6" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4.5999999999999996</v>
       </c>
@@ -840,18 +942,18 @@
       <c r="E7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="K7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="24">
+      <c r="L7" s="26">
         <v>50</v>
       </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -867,30 +969,33 @@
       <c r="E8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="G8" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="7">
-        <f>I4/I7</f>
+      <c r="L8" s="31">
+        <f>L4/L7</f>
         <v>5.0059999999999993</v>
       </c>
-      <c r="J8" s="7">
-        <f>J4/I7</f>
+      <c r="M8" s="31">
+        <f>M4/L7</f>
         <v>3.4180000000000006</v>
       </c>
-      <c r="K8" s="7">
-        <f>K4/I7</f>
+      <c r="N8" s="31">
+        <f>N4/L7</f>
         <v>1.464</v>
       </c>
-      <c r="L8" s="7">
-        <f>L4/I7</f>
+      <c r="O8" s="31">
+        <f>O4/L7</f>
         <v>0.24399999999999991</v>
       </c>
-      <c r="M8" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P8" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4.4000000000000004</v>
       </c>
@@ -906,28 +1011,31 @@
       <c r="E9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="7">
-        <f>I5/I7</f>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="28"/>
+      <c r="L9" s="31">
+        <f>L5/L7</f>
         <v>5.9359999999999999</v>
       </c>
-      <c r="J9" s="7">
-        <f>J5/I7</f>
+      <c r="M9" s="31">
+        <f>M5/L7</f>
         <v>2.7700000000000005</v>
       </c>
-      <c r="K9" s="7">
-        <f>K5/I7</f>
+      <c r="N9" s="31">
+        <f>N5/L7</f>
         <v>4.26</v>
       </c>
-      <c r="L9" s="7">
-        <f>L5/I7</f>
+      <c r="O9" s="31">
+        <f>O5/L7</f>
         <v>1.3259999999999998</v>
       </c>
-      <c r="M9" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P9" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4.9000000000000004</v>
       </c>
@@ -943,28 +1051,31 @@
       <c r="E10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="7">
-        <f>I6/I7</f>
+      <c r="G10" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="29"/>
+      <c r="L10" s="31">
+        <f>L6/L7</f>
         <v>6.5879999999999983</v>
       </c>
-      <c r="J10" s="7">
-        <f>J6/I7</f>
+      <c r="M10" s="31">
+        <f>M6/L7</f>
         <v>2.9739999999999998</v>
       </c>
-      <c r="K10" s="7">
-        <f>K6/I7</f>
+      <c r="N10" s="31">
+        <f>N6/L7</f>
         <v>5.5519999999999996</v>
       </c>
-      <c r="L10" s="7">
-        <f>L6/I7</f>
+      <c r="O10" s="31">
+        <f>O6/L7</f>
         <v>2.0519999999999996</v>
       </c>
-      <c r="M10" s="12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P10" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>5.4</v>
       </c>
@@ -981,7 +1092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4.8</v>
       </c>
@@ -998,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4.8</v>
       </c>
@@ -1014,23 +1125,26 @@
       <c r="E13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="22">
-        <v>6.2</v>
-      </c>
-      <c r="J13" s="22">
-        <v>2.8</v>
-      </c>
-      <c r="K13" s="22">
-        <v>4.8</v>
-      </c>
       <c r="L13" s="22">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="M13" s="22">
+        <v>8</v>
+      </c>
+      <c r="N13" s="22">
+        <v>9</v>
+      </c>
+      <c r="O13" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>4.3</v>
       </c>
@@ -1046,12 +1160,12 @@
       <c r="E14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>5.8</v>
       </c>
@@ -1067,11 +1181,14 @@
       <c r="E15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="M15" s="29" t="s">
+      <c r="G15" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="P15" s="24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>5.7</v>
       </c>
@@ -1087,31 +1204,34 @@
       <c r="E16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="G16" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="15" t="s">
         <v>8</v>
-      </c>
-      <c r="I16" s="7">
-        <f>(I8-I13)^2</f>
-        <v>1.4256360000000019</v>
-      </c>
-      <c r="J16" s="7">
-        <f>(J8-J13)^2</f>
-        <v>0.38192400000000093</v>
-      </c>
-      <c r="K16" s="7">
-        <f>(K8-K13)^2</f>
-        <v>11.128895999999999</v>
       </c>
       <c r="L16" s="7">
         <f>(L8-L13)^2</f>
-        <v>2.4211360000000002</v>
-      </c>
-      <c r="M16" s="17">
-        <f>SQRT(I16+J16+K16+L16)</f>
-        <v>3.9188763695732991</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.5999999999992073E-5</v>
+      </c>
+      <c r="M16" s="7">
+        <f>(M8-M13)^2</f>
+        <v>20.994723999999991</v>
+      </c>
+      <c r="N16" s="7">
+        <f>(N8-N13)^2</f>
+        <v>56.791295999999996</v>
+      </c>
+      <c r="O16" s="7">
+        <f>(O8-O13)^2</f>
+        <v>3.0835360000000001</v>
+      </c>
+      <c r="P16" s="17">
+        <f>SQRT(L16+M16+N16+O16)</f>
+        <v>8.992752192738326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>5.4</v>
       </c>
@@ -1127,31 +1247,34 @@
       <c r="E17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="G17" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="14" t="s">
         <v>9</v>
-      </c>
-      <c r="I17" s="7">
-        <f>(I9-I13)^2</f>
-        <v>6.9696000000000119E-2</v>
-      </c>
-      <c r="J17" s="7">
-        <f>(J9-J13)^2</f>
-        <v>8.9999999999996159E-4</v>
-      </c>
-      <c r="K17" s="7">
-        <f>(K9-K13)^2</f>
-        <v>0.29160000000000003</v>
       </c>
       <c r="L17" s="7">
         <f>(L9-L13)^2</f>
-        <v>0.22467600000000018</v>
-      </c>
-      <c r="M17" s="17">
-        <f>SQRT(I17+J17+K17+L17)</f>
-        <v>0.76607571427372656</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.87609599999999987</v>
+      </c>
+      <c r="M17" s="7">
+        <f>(M9-M13)^2</f>
+        <v>27.352899999999995</v>
+      </c>
+      <c r="N17" s="7">
+        <f>(N9-N13)^2</f>
+        <v>22.467600000000001</v>
+      </c>
+      <c r="O17" s="7">
+        <f>(O9-O13)^2</f>
+        <v>0.45427600000000024</v>
+      </c>
+      <c r="P17" s="17">
+        <f>SQRT(L17+M17+N17+O17)</f>
+        <v>7.1519837807422357</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -1167,31 +1290,34 @@
       <c r="E18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="G18" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="16" t="s">
         <v>10</v>
-      </c>
-      <c r="I18" s="7">
-        <f>(I10-I13)^2</f>
-        <v>0.15054399999999854</v>
-      </c>
-      <c r="J18" s="7">
-        <f>(J10-J13)^2</f>
-        <v>3.0275999999999977E-2</v>
-      </c>
-      <c r="K18" s="7">
-        <f>(K10-K13)^2</f>
-        <v>0.56550399999999967</v>
       </c>
       <c r="L18" s="7">
         <f>(L10-L13)^2</f>
-        <v>6.3503999999999783E-2</v>
-      </c>
-      <c r="M18" s="17">
-        <f>SQRT(I18+J18+K18+L18)</f>
-        <v>0.89990443937120235</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2.5217439999999947</v>
+      </c>
+      <c r="M18" s="7">
+        <f>(M10-M13)^2</f>
+        <v>25.260675999999997</v>
+      </c>
+      <c r="N18" s="7">
+        <f>(N10-N13)^2</f>
+        <v>11.888704000000002</v>
+      </c>
+      <c r="O18" s="7">
+        <f>(O10-O13)^2</f>
+        <v>2.7039999999999586E-3</v>
+      </c>
+      <c r="P18" s="17">
+        <f>SQRT(L18+M18+N18+O18)</f>
+        <v>6.2987163771676524</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>5.7</v>
       </c>
@@ -1207,8 +1333,11 @@
       <c r="E19" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="G19" s="39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -1224,15 +1353,15 @@
       <c r="E20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L20" s="18" t="s">
+      <c r="O20" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="M20" s="19">
-        <f>MIN(M16:M18)</f>
-        <v>0.76607571427372656</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P20" s="19">
+        <f>MIN(P16:P18)</f>
+        <v>6.2987163771676524</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>5.4</v>
       </c>
@@ -1248,15 +1377,18 @@
       <c r="E21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L21" s="18" t="s">
+      <c r="I21" t="s">
+        <v>24</v>
+      </c>
+      <c r="O21" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="7" t="str">
-        <f>IF(EXACT(M20,M16),H16,IF(EXACT(M20,M17),H17,IF(EXACT(M20,M18),H18,"Ninguno")))</f>
-        <v>Distancia versicolor</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P21" s="7" t="str">
+        <f>IF(EXACT(P20,P16),K16,IF(EXACT(P20,P17),K17,IF(EXACT(P20,P18),K18,"Ninguno")))</f>
+        <v>Distancia virginica</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -1273,7 +1405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>4.5999999999999996</v>
       </c>
@@ -1289,8 +1421,20 @@
       <c r="E23" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I23" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="L23" s="36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -1306,12 +1450,15 @@
       <c r="E24" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I24" s="20"/>
+      <c r="H24" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="37"/>
       <c r="J24" s="20"/>
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>4.8</v>
       </c>
@@ -1327,8 +1474,20 @@
       <c r="E25" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H25" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25" s="38">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>5</v>
       </c>
@@ -1344,8 +1503,12 @@
       <c r="E26" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H26" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="38"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>5</v>
       </c>
@@ -1361,8 +1524,12 @@
       <c r="E27" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H27" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27" s="38"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>5.2</v>
       </c>
@@ -1379,7 +1546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>5.2</v>
       </c>
@@ -1396,7 +1563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>4.7</v>
       </c>
@@ -1413,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>4.8</v>
       </c>
@@ -1430,7 +1597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>5.4</v>
       </c>
@@ -3455,14 +3622,14 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="K8:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I4:L6" formulaRange="1"/>
+    <ignoredError sqref="L4:O6" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>